<commit_message>
towards first csc computation
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB04FF7-0472-4848-83BD-F8A4222BDB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA97137C-EE14-4283-8153-215B9391DC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11925" yWindow="8100" windowWidth="24600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
params 1-6 get best ini zeta
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA97137C-EE14-4283-8153-215B9391DC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7379832B-490C-4856-A4B8-C47AFB623090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,30 +495,156 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.3</v>
+      </c>
+      <c r="C3">
+        <v>-0.4</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>1.5</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+      <c r="C4">
+        <v>-0.4</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>1.5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0.3</v>
+      </c>
+      <c r="C5">
+        <v>-0.1</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>0.3</v>
+      </c>
+      <c r="C6">
+        <v>-0.1</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>1.5</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.3</v>
+      </c>
+      <c r="C7">
+        <v>-0.6</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>1.5</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.3</v>
+      </c>
+      <c r="C8">
+        <v>-0.6</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>1.5</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added S curves from water retention characteristics
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87702AE8-9C8D-4A27-A1CC-A57E484A9AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9CCFC0-DE4F-4153-AFA0-CC499915995C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A31"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,16 +496,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C3">
-        <v>-0.4</v>
+        <v>-0.35</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <v>1.5</v>
@@ -522,16 +522,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
-        <v>-0.4</v>
+        <v>-0.35</v>
       </c>
       <c r="D4">
         <v>100</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>1.5</v>
@@ -548,10 +548,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
-        <v>-0.1</v>
+        <v>-0.35</v>
       </c>
       <c r="D5">
         <v>100</v>
@@ -574,16 +574,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C6">
-        <v>-0.1</v>
+        <v>-0.35</v>
       </c>
       <c r="D6">
         <v>100</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>1.5</v>
@@ -600,16 +600,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C7">
-        <v>-0.6</v>
+        <v>-0.35</v>
       </c>
       <c r="D7">
         <v>100</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>1.5</v>
@@ -626,16 +626,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C8">
-        <v>-0.6</v>
+        <v>-0.35</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>1.5</v>

</xml_diff>

<commit_message>
goal: compute best zeta in csc
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\blopti_dev\winrock_calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38826C4E-1519-46B6-A9DD-9025BF4ECC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831754AC-AA58-4C43-9871-9A890894A571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11745" yWindow="1740" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,12 +123,48 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,8 +179,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,15 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -466,185 +508,699 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0.2</v>
-      </c>
-      <c r="C2">
-        <v>-0.35</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>1.5</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="B2" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.1</v>
-      </c>
-      <c r="C3">
-        <v>-0.35</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="F3">
-        <v>1.5</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.1</v>
-      </c>
-      <c r="C4">
-        <v>-0.35</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4">
+      <c r="B6" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>80</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>80</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="F4">
-        <v>1.5</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0.1</v>
-      </c>
-      <c r="C5">
-        <v>-0.35</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5">
+      <c r="B8" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>80</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="F5">
-        <v>1.5</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0.1</v>
-      </c>
-      <c r="C6">
-        <v>-0.35</v>
-      </c>
-      <c r="D6">
-        <v>100</v>
-      </c>
-      <c r="E6">
+      <c r="B9" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>80</v>
+      </c>
+      <c r="E9" s="2">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="F6">
-        <v>1.5</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0.1</v>
-      </c>
-      <c r="C7">
-        <v>-0.35</v>
-      </c>
-      <c r="D7">
-        <v>100</v>
-      </c>
-      <c r="E7">
+      <c r="B10" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>500</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="F7">
-        <v>1.5</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>0.1</v>
-      </c>
-      <c r="C8">
-        <v>-0.35</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>1.5</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
+      <c r="B11" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>500</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>500</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>500</v>
+      </c>
+      <c r="E13" s="3">
+        <v>10</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G13" s="3">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="4">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="4">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="4">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G17" s="4">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="5">
+        <v>80</v>
+      </c>
+      <c r="E18" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="G18" s="5">
+        <v>5</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>80</v>
+      </c>
+      <c r="E19" s="5">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="G19" s="5">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>80</v>
+      </c>
+      <c r="E20" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="G20" s="5">
+        <v>5</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>80</v>
+      </c>
+      <c r="E21" s="5">
+        <v>10</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="G21" s="5">
+        <v>5</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="6">
+        <v>500</v>
+      </c>
+      <c r="E22" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="G22" s="6">
+        <v>5</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1</v>
+      </c>
+      <c r="I22" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="6">
+        <v>500</v>
+      </c>
+      <c r="E23" s="6">
+        <v>5</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="G23" s="6">
+        <v>5</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1</v>
+      </c>
+      <c r="I23" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="6">
+        <v>500</v>
+      </c>
+      <c r="E24" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="G24" s="6">
+        <v>5</v>
+      </c>
+      <c r="H24" s="6">
+        <v>1</v>
+      </c>
+      <c r="I24" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="6">
+        <v>500</v>
+      </c>
+      <c r="E25" s="6">
+        <v>10</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="G25" s="6">
+        <v>5</v>
+      </c>
+      <c r="H25" s="6">
+        <v>1</v>
+      </c>
+      <c r="I25" s="6">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some plots and some comments in math_diff_wave
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03304AC-05BC-446C-BBFD-731AF3237950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A9F814-2278-404E-A04F-F37B9D5BB18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +133,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,9 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG14" sqref="AG14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,16 +498,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="C2" s="1">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="1">
-        <v>68.53</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1">
-        <v>18.97</v>
+        <v>2.5</v>
       </c>
       <c r="F2" s="1">
         <v>1.5</v>
@@ -506,16 +527,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="C3" s="1">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="1">
-        <v>286.57</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1">
-        <v>4.54</v>
+        <v>7.5</v>
       </c>
       <c r="F3" s="1">
         <v>1.5</v>
@@ -534,28 +555,173 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D4" s="1">
-        <v>641.66</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="B4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>500</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F4" s="2">
         <v>1.5</v>
       </c>
-      <c r="G4" s="1">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="G4" s="2">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>500</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>50</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>50</v>
+      </c>
+      <c r="E7" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>500</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>5</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>500</v>
+      </c>
+      <c r="E9" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="4">
+        <v>5</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
         <v>1000</v>
       </c>
     </row>

</xml_diff>